<commit_message>
Work on Texture Atlas
Not finished yet.
</commit_message>
<xml_diff>
--- a/DTMS_The_Dungeon/Tile Index.xlsx
+++ b/DTMS_The_Dungeon/Tile Index.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\GitHub\DungeonTiles\DTMS_The_Dungeon\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="7965" activeTab="1"/>
   </bookViews>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="98">
   <si>
     <t>PAGE 1</t>
   </si>
@@ -315,12 +320,15 @@
   </si>
   <si>
     <t>Double Iron Open</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -548,11 +556,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -589,53 +610,83 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -664,35 +715,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,7 +1031,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1011,8 +1042,8 @@
   <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,9 +2454,9 @@
       </c>
     </row>
     <row r="68" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D69" s="4"/>
@@ -2611,10 +2642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM33"/>
+  <dimension ref="A1:AM34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM19" sqref="AM19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2723,325 +2754,349 @@
       <c r="AG1" s="11">
         <v>32</v>
       </c>
-      <c r="AH1" s="11">
-        <v>33</v>
+      <c r="AH1" s="11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="27" t="s">
+      <c r="B2" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="27" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="27" t="s">
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="29"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI2" s="4"/>
     </row>
     <row r="3" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="33"/>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="34"/>
-      <c r="AD3" s="34"/>
-      <c r="AE3" s="34"/>
-      <c r="AF3" s="34"/>
-      <c r="AG3" s="35"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="30"/>
+      <c r="AE3" s="30"/>
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI3" s="4"/>
     </row>
     <row r="4" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="35"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI4" s="4"/>
     </row>
     <row r="5" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="34"/>
-      <c r="AB5" s="34"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="34"/>
-      <c r="AE5" s="34"/>
-      <c r="AF5" s="34"/>
-      <c r="AG5" s="35"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="30"/>
+      <c r="AB5" s="30"/>
+      <c r="AC5" s="30"/>
+      <c r="AD5" s="30"/>
+      <c r="AE5" s="30"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="31"/>
+      <c r="AH5" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI5" s="4"/>
     </row>
     <row r="6" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="33"/>
-      <c r="AA6" s="34"/>
-      <c r="AB6" s="34"/>
-      <c r="AC6" s="34"/>
-      <c r="AD6" s="34"/>
-      <c r="AE6" s="34"/>
-      <c r="AF6" s="34"/>
-      <c r="AG6" s="35"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+      <c r="Y6" s="31"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="30"/>
+      <c r="AB6" s="30"/>
+      <c r="AC6" s="30"/>
+      <c r="AD6" s="30"/>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="30"/>
+      <c r="AG6" s="31"/>
+      <c r="AH6" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI6" s="4"/>
     </row>
     <row r="7" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="33"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="34"/>
-      <c r="AC7" s="34"/>
-      <c r="AD7" s="34"/>
-      <c r="AE7" s="34"/>
-      <c r="AF7" s="34"/>
-      <c r="AG7" s="35"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="30"/>
+      <c r="AE7" s="30"/>
+      <c r="AF7" s="30"/>
+      <c r="AG7" s="31"/>
+      <c r="AH7" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI7" s="4"/>
     </row>
     <row r="8" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="34"/>
-      <c r="V8" s="34"/>
-      <c r="W8" s="34"/>
-      <c r="X8" s="34"/>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="33"/>
-      <c r="AA8" s="34"/>
-      <c r="AB8" s="34"/>
-      <c r="AC8" s="34"/>
-      <c r="AD8" s="34"/>
-      <c r="AE8" s="34"/>
-      <c r="AF8" s="34"/>
-      <c r="AG8" s="35"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="30"/>
+      <c r="X8" s="30"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="30"/>
+      <c r="AB8" s="30"/>
+      <c r="AC8" s="30"/>
+      <c r="AD8" s="30"/>
+      <c r="AE8" s="30"/>
+      <c r="AF8" s="30"/>
+      <c r="AG8" s="31"/>
+      <c r="AH8" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI8" s="4"/>
     </row>
     <row r="9" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="31"/>
-      <c r="AB9" s="31"/>
-      <c r="AC9" s="31"/>
-      <c r="AD9" s="31"/>
-      <c r="AE9" s="31"/>
-      <c r="AF9" s="31"/>
-      <c r="AG9" s="32"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="27"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI9" s="4"/>
-      <c r="AJ9" s="53"/>
-      <c r="AK9" s="53"/>
-      <c r="AL9" s="53"/>
-      <c r="AM9" s="53"/>
+      <c r="AJ9" s="20"/>
+      <c r="AK9" s="20"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="20"/>
     </row>
     <row r="10" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
@@ -3071,40 +3126,43 @@
       <c r="I10" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="21" t="s">
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="21" t="s">
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="27" t="s">
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="W10" s="28"/>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="27" t="s">
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AA10" s="28"/>
-      <c r="AB10" s="28"/>
-      <c r="AC10" s="28"/>
-      <c r="AD10" s="28"/>
-      <c r="AE10" s="28"/>
-      <c r="AF10" s="28"/>
-      <c r="AG10" s="29"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI10" s="4"/>
     </row>
     <row r="11" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3135,30 +3193,33 @@
       <c r="I11" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="34"/>
-      <c r="X11" s="34"/>
-      <c r="Y11" s="35"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="34"/>
-      <c r="AB11" s="34"/>
-      <c r="AC11" s="34"/>
-      <c r="AD11" s="34"/>
-      <c r="AE11" s="34"/>
-      <c r="AF11" s="34"/>
-      <c r="AG11" s="35"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="31"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="30"/>
+      <c r="AE11" s="30"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="31"/>
+      <c r="AH11" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI11" s="4"/>
     </row>
     <row r="12" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3171,93 +3232,99 @@
       <c r="C12" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="49" t="s">
+      <c r="E12" s="25"/>
+      <c r="F12" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="50"/>
-      <c r="H12" s="21" t="s">
+      <c r="G12" s="43"/>
+      <c r="H12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="21" t="s">
+      <c r="I12" s="33"/>
+      <c r="J12" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="21" t="s">
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="33"/>
-      <c r="W12" s="34"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="33"/>
-      <c r="AA12" s="34"/>
-      <c r="AB12" s="34"/>
-      <c r="AC12" s="34"/>
-      <c r="AD12" s="34"/>
-      <c r="AE12" s="34"/>
-      <c r="AF12" s="34"/>
-      <c r="AG12" s="35"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="30"/>
+      <c r="AD12" s="30"/>
+      <c r="AE12" s="30"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="31"/>
+      <c r="AH12" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI12" s="4"/>
     </row>
     <row r="13" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="31"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="33"/>
-      <c r="AA13" s="34"/>
-      <c r="AB13" s="34"/>
-      <c r="AC13" s="34"/>
-      <c r="AD13" s="34"/>
-      <c r="AE13" s="34"/>
-      <c r="AF13" s="34"/>
-      <c r="AG13" s="35"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="30"/>
+      <c r="AE13" s="30"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="31"/>
+      <c r="AH13" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI13" s="4"/>
-      <c r="AJ13" s="53"/>
-      <c r="AK13" s="53"/>
-      <c r="AL13" s="53"/>
-      <c r="AM13" s="53"/>
+      <c r="AJ13" s="20"/>
+      <c r="AK13" s="20"/>
+      <c r="AL13" s="20"/>
+      <c r="AM13" s="20"/>
     </row>
     <row r="14" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
@@ -3275,46 +3342,49 @@
       <c r="E14" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="27" t="s">
+      <c r="G14" s="25"/>
+      <c r="H14" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="28"/>
-      <c r="J14" s="27" t="s">
+      <c r="I14" s="24"/>
+      <c r="J14" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="21" t="s">
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="27" t="s">
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="W14" s="28"/>
-      <c r="X14" s="28"/>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="33"/>
-      <c r="AA14" s="34"/>
-      <c r="AB14" s="34"/>
-      <c r="AC14" s="34"/>
-      <c r="AD14" s="34"/>
-      <c r="AE14" s="34"/>
-      <c r="AF14" s="34"/>
-      <c r="AG14" s="35"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="29"/>
+      <c r="AA14" s="30"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="30"/>
+      <c r="AD14" s="30"/>
+      <c r="AE14" s="30"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="31"/>
+      <c r="AH14" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI14" s="4"/>
     </row>
     <row r="15" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3333,749 +3403,770 @@
       <c r="E15" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="34"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="33"/>
-      <c r="AA15" s="34"/>
-      <c r="AB15" s="34"/>
-      <c r="AC15" s="34"/>
-      <c r="AD15" s="34"/>
-      <c r="AE15" s="34"/>
-      <c r="AF15" s="34"/>
-      <c r="AG15" s="35"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="31"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="30"/>
+      <c r="AB15" s="30"/>
+      <c r="AC15" s="30"/>
+      <c r="AD15" s="30"/>
+      <c r="AE15" s="30"/>
+      <c r="AF15" s="30"/>
+      <c r="AG15" s="31"/>
+      <c r="AH15" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI15" s="4"/>
-      <c r="AJ15" s="53"/>
-      <c r="AK15" s="53"/>
-      <c r="AL15" s="53"/>
-      <c r="AM15" s="53"/>
+      <c r="AJ15" s="20"/>
+      <c r="AK15" s="20"/>
+      <c r="AL15" s="20"/>
+      <c r="AM15" s="20"/>
     </row>
     <row r="16" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="48"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="17" t="s">
         <v>91</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="33"/>
+      <c r="H16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="27" t="s">
+      <c r="I16" s="33"/>
+      <c r="J16" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="27" t="s">
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="34"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="33"/>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="34"/>
-      <c r="AC16" s="34"/>
-      <c r="AD16" s="34"/>
-      <c r="AE16" s="34"/>
-      <c r="AF16" s="34"/>
-      <c r="AG16" s="35"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="30"/>
+      <c r="AB16" s="30"/>
+      <c r="AC16" s="30"/>
+      <c r="AD16" s="30"/>
+      <c r="AE16" s="30"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="31"/>
+      <c r="AH16" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI16" s="4"/>
-      <c r="AJ16" s="53"/>
-      <c r="AK16" s="53"/>
-      <c r="AL16" s="53"/>
-      <c r="AM16" s="53"/>
     </row>
     <row r="17" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47" t="s">
+      <c r="C17" s="37"/>
+      <c r="D17" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="31"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="30"/>
-      <c r="AA17" s="31"/>
-      <c r="AB17" s="31"/>
-      <c r="AC17" s="31"/>
-      <c r="AD17" s="31"/>
-      <c r="AE17" s="31"/>
-      <c r="AF17" s="31"/>
-      <c r="AG17" s="32"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="27"/>
+      <c r="AB17" s="27"/>
+      <c r="AC17" s="27"/>
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="27"/>
+      <c r="AF17" s="27"/>
+      <c r="AG17" s="28"/>
+      <c r="AH17" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI17" s="4"/>
-      <c r="AJ17" s="53"/>
-      <c r="AK17" s="53"/>
-      <c r="AL17" s="53"/>
-      <c r="AM17" s="53"/>
     </row>
     <row r="18" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>17</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="21" t="s">
+      <c r="C18" s="33"/>
+      <c r="D18" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="27" t="s">
+      <c r="E18" s="33"/>
+      <c r="H18" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="I18" s="29"/>
-      <c r="J18" s="21" t="s">
+      <c r="I18" s="25"/>
+      <c r="J18" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="K18" s="23"/>
-      <c r="L18" s="27" t="s">
+      <c r="K18" s="33"/>
+      <c r="L18" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M18" s="29"/>
-      <c r="N18" s="27" t="s">
+      <c r="M18" s="25"/>
+      <c r="N18" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="27" t="s">
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="W18" s="28"/>
-      <c r="X18" s="28"/>
-      <c r="Y18" s="29"/>
-      <c r="Z18" s="27" t="s">
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="25"/>
+      <c r="Z18" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="AA18" s="28"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="28"/>
-      <c r="AE18" s="28"/>
-      <c r="AF18" s="28"/>
-      <c r="AG18" s="29"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="24"/>
+      <c r="AG18" s="25"/>
+      <c r="AH18" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI18" s="4"/>
-      <c r="AJ18" s="53"/>
-      <c r="AK18" s="53"/>
-      <c r="AL18" s="53"/>
-      <c r="AM18" s="53"/>
+      <c r="AJ18" s="20"/>
+      <c r="AK18" s="20"/>
+      <c r="AL18" s="20"/>
+      <c r="AM18" s="20"/>
     </row>
     <row r="19" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="30"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="31"/>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="33"/>
-      <c r="AA19" s="34"/>
-      <c r="AB19" s="34"/>
-      <c r="AC19" s="34"/>
-      <c r="AD19" s="34"/>
-      <c r="AE19" s="34"/>
-      <c r="AF19" s="34"/>
-      <c r="AG19" s="35"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="30"/>
+      <c r="AB19" s="30"/>
+      <c r="AC19" s="30"/>
+      <c r="AD19" s="30"/>
+      <c r="AE19" s="30"/>
+      <c r="AF19" s="30"/>
+      <c r="AG19" s="31"/>
+      <c r="AH19" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI19" s="4"/>
-      <c r="AJ19" s="53"/>
-      <c r="AK19" s="53"/>
-      <c r="AL19" s="53"/>
-      <c r="AM19" s="53"/>
+      <c r="AJ19" s="20"/>
+      <c r="AK19" s="20"/>
+      <c r="AL19" s="20"/>
+      <c r="AM19" s="20"/>
     </row>
     <row r="20" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>19</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="27" t="s">
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="27" t="s">
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
-      <c r="V20" s="28"/>
-      <c r="W20" s="28"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="34"/>
-      <c r="AB20" s="34"/>
-      <c r="AC20" s="34"/>
-      <c r="AD20" s="34"/>
-      <c r="AE20" s="34"/>
-      <c r="AF20" s="34"/>
-      <c r="AG20" s="35"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="30"/>
+      <c r="AB20" s="30"/>
+      <c r="AC20" s="30"/>
+      <c r="AD20" s="30"/>
+      <c r="AE20" s="30"/>
+      <c r="AF20" s="30"/>
+      <c r="AG20" s="31"/>
+      <c r="AH20" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI20" s="4"/>
-      <c r="AJ20" s="53"/>
-      <c r="AK20" s="53"/>
-      <c r="AL20" s="53"/>
-      <c r="AM20" s="53"/>
+      <c r="AJ20" s="20"/>
+      <c r="AK20" s="20"/>
+      <c r="AL20" s="20"/>
+      <c r="AM20" s="20"/>
     </row>
     <row r="21" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="31"/>
-      <c r="X21" s="31"/>
-      <c r="Y21" s="32"/>
-      <c r="Z21" s="33"/>
-      <c r="AA21" s="34"/>
-      <c r="AB21" s="34"/>
-      <c r="AC21" s="34"/>
-      <c r="AD21" s="34"/>
-      <c r="AE21" s="34"/>
-      <c r="AF21" s="34"/>
-      <c r="AG21" s="35"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="30"/>
+      <c r="AB21" s="30"/>
+      <c r="AC21" s="30"/>
+      <c r="AD21" s="30"/>
+      <c r="AE21" s="30"/>
+      <c r="AF21" s="30"/>
+      <c r="AG21" s="31"/>
+      <c r="AH21" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI21" s="4"/>
-      <c r="AJ21" s="53"/>
-      <c r="AK21" s="53"/>
-      <c r="AL21" s="53"/>
-      <c r="AM21" s="53"/>
+      <c r="AJ21" s="20"/>
+      <c r="AK21" s="20"/>
+      <c r="AL21" s="20"/>
+      <c r="AM21" s="20"/>
     </row>
     <row r="22" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>21</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="27" t="s">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="27" t="s">
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="27" t="s">
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="29"/>
-      <c r="V22" s="27" t="s">
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="25"/>
+      <c r="V22" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="33"/>
-      <c r="AA22" s="34"/>
-      <c r="AB22" s="34"/>
-      <c r="AC22" s="34"/>
-      <c r="AD22" s="34"/>
-      <c r="AE22" s="34"/>
-      <c r="AF22" s="34"/>
-      <c r="AG22" s="35"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="25"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="30"/>
+      <c r="AB22" s="30"/>
+      <c r="AC22" s="30"/>
+      <c r="AD22" s="30"/>
+      <c r="AE22" s="30"/>
+      <c r="AF22" s="30"/>
+      <c r="AG22" s="31"/>
+      <c r="AH22" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI22" s="4"/>
-      <c r="AJ22" s="53"/>
-      <c r="AK22" s="53"/>
-      <c r="AL22" s="53"/>
-      <c r="AM22" s="53"/>
+      <c r="AJ22" s="20"/>
+      <c r="AK22" s="20"/>
+      <c r="AL22" s="20"/>
+      <c r="AM22" s="20"/>
     </row>
     <row r="23" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>22</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="33"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="33"/>
-      <c r="W23" s="34"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="35"/>
-      <c r="Z23" s="33"/>
-      <c r="AA23" s="34"/>
-      <c r="AB23" s="34"/>
-      <c r="AC23" s="34"/>
-      <c r="AD23" s="34"/>
-      <c r="AE23" s="34"/>
-      <c r="AF23" s="34"/>
-      <c r="AG23" s="35"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="29"/>
+      <c r="AA23" s="30"/>
+      <c r="AB23" s="30"/>
+      <c r="AC23" s="30"/>
+      <c r="AD23" s="30"/>
+      <c r="AE23" s="30"/>
+      <c r="AF23" s="30"/>
+      <c r="AG23" s="31"/>
+      <c r="AH23" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="AI23" s="4"/>
     </row>
     <row r="24" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>23</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="33"/>
-      <c r="W24" s="34"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="35"/>
-      <c r="Z24" s="33"/>
-      <c r="AA24" s="34"/>
-      <c r="AB24" s="34"/>
-      <c r="AC24" s="34"/>
-      <c r="AD24" s="34"/>
-      <c r="AE24" s="34"/>
-      <c r="AF24" s="34"/>
-      <c r="AG24" s="35"/>
-      <c r="AJ24" s="53"/>
-      <c r="AK24" s="53"/>
-      <c r="AL24" s="53"/>
-      <c r="AM24" s="53"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="29"/>
+      <c r="AA24" s="30"/>
+      <c r="AB24" s="30"/>
+      <c r="AC24" s="30"/>
+      <c r="AD24" s="30"/>
+      <c r="AE24" s="30"/>
+      <c r="AF24" s="30"/>
+      <c r="AG24" s="31"/>
+      <c r="AH24" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ24" s="20"/>
     </row>
     <row r="25" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="32"/>
-      <c r="V25" s="30"/>
-      <c r="W25" s="31"/>
-      <c r="X25" s="31"/>
-      <c r="Y25" s="32"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="31"/>
-      <c r="AB25" s="31"/>
-      <c r="AC25" s="31"/>
-      <c r="AD25" s="31"/>
-      <c r="AE25" s="31"/>
-      <c r="AF25" s="31"/>
-      <c r="AG25" s="32"/>
-      <c r="AJ25" s="53"/>
-      <c r="AK25" s="53"/>
-      <c r="AL25" s="53"/>
-      <c r="AM25" s="53"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="28"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="27"/>
+      <c r="AB25" s="27"/>
+      <c r="AC25" s="27"/>
+      <c r="AD25" s="27"/>
+      <c r="AE25" s="27"/>
+      <c r="AF25" s="27"/>
+      <c r="AG25" s="28"/>
+      <c r="AH25" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ25" s="20"/>
     </row>
     <row r="26" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>25</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="27" t="s">
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="27" t="s">
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="S26" s="28"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="28"/>
-      <c r="V26" s="29"/>
-      <c r="W26" s="27" t="s">
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="X26" s="28"/>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="28"/>
-      <c r="AA26" s="29"/>
-      <c r="AB26" s="27" t="s">
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24"/>
+      <c r="Z26" s="24"/>
+      <c r="AA26" s="25"/>
+      <c r="AB26" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="AC26" s="28"/>
-      <c r="AD26" s="29"/>
-      <c r="AE26" s="27" t="s">
+      <c r="AC26" s="24"/>
+      <c r="AD26" s="25"/>
+      <c r="AE26" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="AF26" s="28"/>
-      <c r="AG26" s="29"/>
-      <c r="AJ26" s="53"/>
-      <c r="AK26" s="53"/>
-      <c r="AL26" s="53"/>
-      <c r="AM26" s="53"/>
+      <c r="AF26" s="24"/>
+      <c r="AG26" s="25"/>
+      <c r="AH26" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ26" s="20"/>
     </row>
     <row r="27" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>26</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="35"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="34"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="34"/>
-      <c r="V27" s="35"/>
-      <c r="W27" s="33"/>
-      <c r="X27" s="34"/>
-      <c r="Y27" s="34"/>
-      <c r="Z27" s="34"/>
-      <c r="AA27" s="35"/>
-      <c r="AB27" s="33"/>
-      <c r="AC27" s="34"/>
-      <c r="AD27" s="35"/>
-      <c r="AE27" s="33"/>
-      <c r="AF27" s="34"/>
-      <c r="AG27" s="35"/>
-      <c r="AJ27" s="53"/>
-      <c r="AK27" s="53"/>
-      <c r="AL27" s="53"/>
-      <c r="AM27" s="53"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="30"/>
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="30"/>
+      <c r="AA27" s="31"/>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="30"/>
+      <c r="AD27" s="31"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="30"/>
+      <c r="AG27" s="31"/>
+      <c r="AH27" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ27" s="20"/>
     </row>
     <row r="28" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>27</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="33"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="34"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="34"/>
-      <c r="AA28" s="35"/>
-      <c r="AB28" s="30"/>
-      <c r="AC28" s="31"/>
-      <c r="AD28" s="32"/>
-      <c r="AE28" s="30"/>
-      <c r="AF28" s="31"/>
-      <c r="AG28" s="32"/>
-      <c r="AJ28" s="53"/>
-      <c r="AK28" s="53"/>
-      <c r="AL28" s="53"/>
-      <c r="AM28" s="53"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="30"/>
+      <c r="Y28" s="30"/>
+      <c r="Z28" s="30"/>
+      <c r="AA28" s="31"/>
+      <c r="AB28" s="26"/>
+      <c r="AC28" s="27"/>
+      <c r="AD28" s="28"/>
+      <c r="AE28" s="26"/>
+      <c r="AF28" s="27"/>
+      <c r="AG28" s="28"/>
+      <c r="AH28" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ28" s="20"/>
     </row>
     <row r="29" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>28</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="33"/>
-      <c r="S29" s="34"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="33"/>
-      <c r="X29" s="34"/>
-      <c r="Y29" s="34"/>
-      <c r="Z29" s="34"/>
-      <c r="AA29" s="35"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="30"/>
+      <c r="Y29" s="30"/>
+      <c r="Z29" s="30"/>
+      <c r="AA29" s="31"/>
       <c r="AB29" s="19"/>
       <c r="AC29" s="19"/>
       <c r="AD29" s="19"/>
       <c r="AE29" s="19"/>
       <c r="AF29" s="19"/>
       <c r="AG29" s="19"/>
-      <c r="AJ29" s="53"/>
-      <c r="AK29" s="53"/>
-      <c r="AL29" s="53"/>
-      <c r="AM29" s="53"/>
+      <c r="AH29" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ29" s="20"/>
+      <c r="AK29" s="20"/>
+      <c r="AL29" s="20"/>
+      <c r="AM29" s="20"/>
     </row>
     <row r="30" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>29</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="54" t="s">
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="K30" s="17" t="s">
+      <c r="K30" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
+      <c r="L30" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="M30" s="58"/>
       <c r="N30" s="19"/>
       <c r="O30" s="19"/>
       <c r="P30" s="19"/>
       <c r="Q30" s="19"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="31"/>
-      <c r="U30" s="31"/>
-      <c r="V30" s="32"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="31"/>
-      <c r="Z30" s="31"/>
-      <c r="AA30" s="32"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="27"/>
+      <c r="Y30" s="27"/>
+      <c r="Z30" s="27"/>
+      <c r="AA30" s="28"/>
       <c r="AB30" s="18"/>
       <c r="AC30" s="18"/>
       <c r="AD30" s="18"/>
       <c r="AE30" s="18"/>
       <c r="AF30" s="18"/>
       <c r="AG30" s="18"/>
-      <c r="AJ30" s="53"/>
-      <c r="AK30" s="53"/>
-      <c r="AL30" s="53"/>
-      <c r="AM30" s="53"/>
+      <c r="AH30" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ30" s="20"/>
+      <c r="AK30" s="20"/>
+      <c r="AL30" s="20"/>
+      <c r="AM30" s="20"/>
     </row>
     <row r="31" spans="1:39" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="32"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="28"/>
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="57"/>
       <c r="N31" s="19"/>
       <c r="O31" s="19"/>
       <c r="P31" s="19"/>
@@ -4096,10 +4187,13 @@
       <c r="AE31" s="19"/>
       <c r="AF31" s="19"/>
       <c r="AG31" s="19"/>
-      <c r="AJ31" s="53"/>
-      <c r="AK31" s="53"/>
-      <c r="AL31" s="53"/>
-      <c r="AM31" s="53"/>
+      <c r="AH31" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ31" s="20"/>
+      <c r="AK31" s="20"/>
+      <c r="AL31" s="20"/>
+      <c r="AM31" s="20"/>
     </row>
     <row r="32" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
@@ -4137,8 +4231,11 @@
       <c r="AE32" s="19"/>
       <c r="AF32" s="19"/>
       <c r="AG32" s="19"/>
-    </row>
-    <row r="33" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH32" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>32</v>
       </c>
@@ -4174,9 +4271,116 @@
       <c r="AE33" s="19"/>
       <c r="AF33" s="19"/>
       <c r="AG33" s="19"/>
+      <c r="AH33" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="N34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="P34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="R34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="S34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="U34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="V34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="W34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="X34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH34" s="11" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="54">
     <mergeCell ref="B22:I25"/>
     <mergeCell ref="B26:I29"/>
     <mergeCell ref="J26:Q29"/>
@@ -4184,9 +4388,15 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="N16:Q17"/>
-    <mergeCell ref="R16:U17"/>
+    <mergeCell ref="R18:U19"/>
     <mergeCell ref="D12:E13"/>
     <mergeCell ref="F14:G15"/>
+    <mergeCell ref="R26:V30"/>
+    <mergeCell ref="W26:AA30"/>
+    <mergeCell ref="V22:Y25"/>
+    <mergeCell ref="B30:I31"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="H14:I15"/>
     <mergeCell ref="Z2:AG9"/>
     <mergeCell ref="Z10:AG17"/>
     <mergeCell ref="R20:Y21"/>
@@ -4195,43 +4405,36 @@
     <mergeCell ref="L18:M19"/>
     <mergeCell ref="V18:Y19"/>
     <mergeCell ref="N18:Q19"/>
-    <mergeCell ref="R18:U19"/>
+    <mergeCell ref="R12:U13"/>
     <mergeCell ref="J20:Q21"/>
     <mergeCell ref="B20:I21"/>
     <mergeCell ref="Z18:AG25"/>
     <mergeCell ref="J22:M25"/>
     <mergeCell ref="J14:M15"/>
     <mergeCell ref="N22:Q25"/>
-    <mergeCell ref="R26:V30"/>
-    <mergeCell ref="W26:AA30"/>
     <mergeCell ref="B2:I9"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="J16:M17"/>
+    <mergeCell ref="R10:U11"/>
+    <mergeCell ref="R16:U17"/>
+    <mergeCell ref="N14:Q15"/>
+    <mergeCell ref="J10:M11"/>
+    <mergeCell ref="N10:Q11"/>
+    <mergeCell ref="J12:M13"/>
+    <mergeCell ref="N12:Q13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="F16:G17"/>
+    <mergeCell ref="H16:I17"/>
     <mergeCell ref="J2:Q9"/>
     <mergeCell ref="R2:Y9"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="J16:M17"/>
-    <mergeCell ref="R10:U11"/>
     <mergeCell ref="R14:U15"/>
-    <mergeCell ref="N14:Q15"/>
-    <mergeCell ref="V22:Y25"/>
-    <mergeCell ref="J10:M11"/>
-    <mergeCell ref="N10:Q11"/>
-    <mergeCell ref="J12:M13"/>
-    <mergeCell ref="N12:Q13"/>
-    <mergeCell ref="B30:I31"/>
+    <mergeCell ref="V10:Y13"/>
     <mergeCell ref="AB26:AD28"/>
     <mergeCell ref="AE26:AG28"/>
     <mergeCell ref="R22:U25"/>
-    <mergeCell ref="F16:G17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="H14:I15"/>
-    <mergeCell ref="R12:U13"/>
-    <mergeCell ref="V10:Y13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>